<commit_message>
Bug Fixes, few sounds
</commit_message>
<xml_diff>
--- a/Projektfortschritt.xlsx
+++ b/Projektfortschritt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\IdeaProjects\projekt10_PacMan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BF544B-75BC-4156-8E4C-5529CD013E6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700ABDF1-84F7-493D-8ACC-ECEEA65E1B30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3870" yWindow="420" windowWidth="23520" windowHeight="13080" xr2:uid="{2A06745D-B8D8-4E00-B44D-5D896F0FF5C5}"/>
+    <workbookView xWindow="4215" yWindow="765" windowWidth="23520" windowHeight="13080" xr2:uid="{2A06745D-B8D8-4E00-B44D-5D896F0FF5C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Fortschritt" sheetId="1" r:id="rId1"/>
@@ -465,7 +465,7 @@
   <dimension ref="A5:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,7 +479,7 @@
       </c>
       <c r="D5" s="3">
         <f>AVERAGE(A6:A13)</f>
-        <v>0.9375</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -524,7 +524,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>4</v>
@@ -553,12 +553,12 @@
       </c>
       <c r="D14" s="3">
         <f>AVERAGE(A15:A21)</f>
-        <v>0.31428571428571433</v>
+        <v>0.58571428571428574</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
@@ -566,7 +566,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
@@ -590,7 +590,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s">
         <v>12</v>
@@ -615,7 +615,7 @@
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <f>AVERAGE(A6:A21)</f>
-        <v>0.64666666666666672</v>
+        <v>0.77999999999999992</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>17</v>

</xml_diff>